<commit_message>
add firefox test case
</commit_message>
<xml_diff>
--- a/trsr/eulaceura-test-1026/firefox测试报告.xlsx
+++ b/trsr/eulaceura-test-1026/firefox测试报告.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="125">
   <si>
     <t>项目名称：</t>
   </si>
@@ -102,9 +102,6 @@
     <t>是否有正确回显</t>
   </si>
   <si>
-    <t>程龙灿</t>
-  </si>
-  <si>
     <t>不通过</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>书签栏是否增加同步内容</t>
   </si>
   <si>
-    <t>同步失败，其它设备书签栏未能同步</t>
-  </si>
-  <si>
     <t>无网页通知</t>
   </si>
   <si>
@@ -199,84 +193,6 @@
   </si>
   <si>
     <t>登录时弹出提示</t>
-  </si>
-  <si>
-    <t>TC00014</t>
-  </si>
-  <si>
-    <t>TC00015</t>
-  </si>
-  <si>
-    <t>TC00016</t>
-  </si>
-  <si>
-    <t>TC00017</t>
-  </si>
-  <si>
-    <t>TC00018</t>
-  </si>
-  <si>
-    <t>TC00019</t>
-  </si>
-  <si>
-    <t>TC00020</t>
-  </si>
-  <si>
-    <t>TC00021</t>
-  </si>
-  <si>
-    <t>TC00022</t>
-  </si>
-  <si>
-    <t>TC00023</t>
-  </si>
-  <si>
-    <t>TC00024</t>
-  </si>
-  <si>
-    <t>TC00025</t>
-  </si>
-  <si>
-    <t>TC00026</t>
-  </si>
-  <si>
-    <t>TC00027</t>
-  </si>
-  <si>
-    <t>TC00028</t>
-  </si>
-  <si>
-    <t>TC00029</t>
-  </si>
-  <si>
-    <t>TC00030</t>
-  </si>
-  <si>
-    <t>TC00031</t>
-  </si>
-  <si>
-    <t>TC00032</t>
-  </si>
-  <si>
-    <t>TC00033</t>
-  </si>
-  <si>
-    <t>TC00034</t>
-  </si>
-  <si>
-    <t>TC00035</t>
-  </si>
-  <si>
-    <t>TC00036</t>
-  </si>
-  <si>
-    <t>TC00037</t>
-  </si>
-  <si>
-    <t>TC00038</t>
-  </si>
-  <si>
-    <t>TC00039</t>
   </si>
   <si>
     <t>1、点击openeuler搜索栏上的收藏按钮
@@ -301,14 +217,6 @@
   </si>
   <si>
     <t>是否有正确回显</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1、点击桌面terminal图标
-2、输入dnf install firefox后回车
-3、按y键确认
-4、输入dnf install firefox --skip-broken后回车
-5、输入dnf install firefox --nobest后回车</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -560,6 +468,22 @@
   </si>
   <si>
     <t>使用 Eulaceura 22H1 镜像启动</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>nexplorer-3e</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已装好 firefox</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步成功，其它设备书签栏增加同步内容</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -567,7 +491,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +503,8 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -586,12 +512,16 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -604,6 +534,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -682,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -729,24 +666,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -759,20 +711,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,120 +742,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>60325</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>1043940</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>860425</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="图片 19" descr="同步1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="18479135" y="10970260"/>
-          <a:ext cx="983615" cy="787400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>1114425</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>2753995</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>894080</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="图片 20" descr="书签无法同步"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19533235" y="10982960"/>
-          <a:ext cx="1639570" cy="808355"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>1047115</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>1031875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="图片 25" descr="保存密码"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="18466435" y="14996160"/>
-          <a:ext cx="999490" cy="958850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
       <xdr:colOff>102235</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -928,7 +760,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -966,7 +798,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1004,7 +836,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1042,7 +874,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1080,7 +912,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1118,7 +950,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1156,7 +988,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1194,7 +1026,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1232,7 +1064,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1270,7 +1102,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1308,7 +1140,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1328,15 +1160,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>133142</xdr:colOff>
+      <xdr:colOff>220190</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>25401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>965200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>962</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>685800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1346,15 +1178,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17100342" y="13119101"/>
-          <a:ext cx="832058" cy="737561"/>
+          <a:off x="17187390" y="11328401"/>
+          <a:ext cx="745010" cy="660399"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1384,7 +1216,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1422,7 +1254,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1442,19 +1274,133 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>129621</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>63501</xdr:rowOff>
+      <xdr:colOff>53421</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>215902</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>2014225</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>939800</xdr:rowOff>
+      <xdr:colOff>1054100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>20796</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="42" name="图片 41"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17020621" y="647702"/>
+          <a:ext cx="1000679" cy="465294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1082121</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>219076</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>2146300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>50067</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="图片 42"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18049321" y="650876"/>
+          <a:ext cx="1064179" cy="491391"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1651000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>717</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16967200" y="12992101"/>
+          <a:ext cx="1651000" cy="1092916"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1536701</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>2929603</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1193800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1467,8 +1413,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17096821" y="749301"/>
-          <a:ext cx="1884604" cy="876299"/>
+          <a:off x="18503901" y="9080501"/>
+          <a:ext cx="1392902" cy="1079499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1480,19 +1426,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>155021</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1016001</xdr:rowOff>
+      <xdr:colOff>241302</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>254001</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>2603501</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>2146602</xdr:rowOff>
+      <xdr:colOff>1374168</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1079500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="图片 42"/>
+        <xdr:cNvPr id="5" name="图片 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1505,8 +1451,101 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17122221" y="1701801"/>
-          <a:ext cx="2448480" cy="1130601"/>
+          <a:off x="17208502" y="9220201"/>
+          <a:ext cx="1132866" cy="825499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1498601</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>2754746</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>901701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="图片 44"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="18465801" y="12103101"/>
+          <a:ext cx="1256145" cy="863600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>50801</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>26510</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>878861</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17018001" y="12091510"/>
+          <a:ext cx="1244599" cy="852351"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1561,7 +1600,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1596,7 +1635,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1807,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4:S16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1840,55 +1879,55 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
     </row>
     <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
     </row>
     <row r="3" spans="1:21" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1955,100 +1994,100 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>91</v>
+      <c r="D4" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="10" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="N4" s="13"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="22">
+      <c r="O4" s="26"/>
+      <c r="P4" s="27">
         <v>44861</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="22">
-        <v>44833</v>
+        <v>61</v>
+      </c>
+      <c r="S4" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="T4" s="27">
+        <v>44861</v>
       </c>
       <c r="U4" s="15"/>
     </row>
     <row r="5" spans="1:21" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="10" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="29"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="10" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
+        <v>69</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
       <c r="J5" s="14" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="10" t="s">
         <v>25</v>
       </c>
       <c r="N5" s="10"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="23"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="28"/>
       <c r="Q5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="S5" s="20"/>
-      <c r="T5" s="23"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="28"/>
       <c r="U5" s="11"/>
     </row>
     <row r="6" spans="1:21" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2056,1109 +2095,537 @@
         <v>2</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="10" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+        <v>74</v>
+      </c>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="14" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="N6" s="10"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="23"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="28"/>
       <c r="Q6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="S6" s="20"/>
-      <c r="T6" s="23"/>
+        <v>28</v>
+      </c>
+      <c r="S6" s="22"/>
+      <c r="T6" s="28"/>
       <c r="U6" s="11"/>
     </row>
     <row r="7" spans="1:21" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="21">
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="19" t="s">
-        <v>106</v>
+      <c r="D7" s="21" t="s">
+        <v>77</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
+        <v>79</v>
+      </c>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
       <c r="J7" s="14" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="N7" s="10"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="R7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="S7" s="20"/>
-      <c r="T7" s="23"/>
+        <v>28</v>
+      </c>
+      <c r="S7" s="22"/>
+      <c r="T7" s="28"/>
       <c r="U7" s="11"/>
     </row>
     <row r="8" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="10" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="20"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="10" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="26" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="N8" s="10"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="R8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="S8" s="20"/>
-      <c r="T8" s="23"/>
+        <v>28</v>
+      </c>
+      <c r="S8" s="22"/>
+      <c r="T8" s="28"/>
       <c r="U8" s="11"/>
     </row>
     <row r="9" spans="1:21" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="10" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="20"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="10" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
+        <v>87</v>
+      </c>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
       <c r="J9" s="14" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="N9" s="10"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="23"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="28"/>
       <c r="Q9" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R9" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="S9" s="20"/>
-      <c r="T9" s="23"/>
+        <v>28</v>
+      </c>
+      <c r="S9" s="22"/>
+      <c r="T9" s="28"/>
       <c r="U9" s="11"/>
     </row>
     <row r="10" spans="1:21" ht="123.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="10" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="20"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="10" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="26" t="s">
-        <v>121</v>
+        <v>91</v>
+      </c>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="K10" s="11"/>
       <c r="L10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="N10" s="10"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="10" t="s">
+      <c r="R10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="22"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="11"/>
+    </row>
+    <row r="11" spans="1:21" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="R10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="S10" s="20"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="11"/>
-    </row>
-    <row r="11" spans="1:21" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="10" t="s">
+      <c r="M11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="10"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="S11" s="22"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="11"/>
+    </row>
+    <row r="12" spans="1:21" s="2" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="K12" s="33"/>
+      <c r="L12" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="31"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="R12" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="13" t="s">
+      <c r="S12" s="23"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="9"/>
+    </row>
+    <row r="13" spans="1:21" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="R11" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="S11" s="20"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="11"/>
-    </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N12" s="13"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="R12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S12" s="21"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="9"/>
-    </row>
-    <row r="13" spans="1:21" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>115</v>
-      </c>
       <c r="G13" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
+        <v>103</v>
+      </c>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
       <c r="J13" s="14" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="10"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="M13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="R13" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="S13" s="20"/>
-      <c r="T13" s="23"/>
+        <v>28</v>
+      </c>
+      <c r="S13" s="22"/>
+      <c r="T13" s="28"/>
       <c r="U13" s="11"/>
     </row>
     <row r="14" spans="1:21" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="13" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C14" s="9"/>
-      <c r="D14" s="20"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="13" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
+        <v>108</v>
+      </c>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
       <c r="J14" s="12" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N14" s="13"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="M14" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N14" s="13"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="R14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S14" s="21"/>
-      <c r="T14" s="24"/>
+        <v>26</v>
+      </c>
+      <c r="S14" s="23"/>
+      <c r="T14" s="29"/>
       <c r="U14" s="9"/>
     </row>
     <row r="15" spans="1:21" s="2" customFormat="1" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="13" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="13" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
+        <v>112</v>
+      </c>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
       <c r="J15" s="12" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="M15" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="N15" s="13"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="24"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="29"/>
       <c r="Q15" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S15" s="21"/>
-      <c r="T15" s="24"/>
+        <v>26</v>
+      </c>
+      <c r="S15" s="23"/>
+      <c r="T15" s="29"/>
       <c r="U15" s="9"/>
     </row>
     <row r="16" spans="1:21" ht="86.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="10" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="18"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="10" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
+        <v>116</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
       <c r="J16" s="14" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="K16" s="11"/>
       <c r="L16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="N16" s="11"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="M16" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N16" s="11"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="10" t="s">
-        <v>58</v>
-      </c>
       <c r="R16" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="S16" s="18"/>
-      <c r="T16" s="25"/>
+        <v>28</v>
+      </c>
+      <c r="S16" s="24"/>
+      <c r="T16" s="30"/>
       <c r="U16" s="11"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="11"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
-      <c r="T34" s="11"/>
-      <c r="U34" s="11"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="11"/>
-      <c r="U35" s="11"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="11"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
-      <c r="T38" s="11"/>
-      <c r="U38" s="11"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-      <c r="T39" s="11"/>
-      <c r="U39" s="11"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-      <c r="T40" s="11"/>
-      <c r="U40" s="11"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="11"/>
-      <c r="U41" s="11"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-      <c r="T42" s="11"/>
-      <c r="U42" s="11"/>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:U42"/>

</xml_diff>